<commit_message>
Poprawki dotyczace klasyfikatora histogramowego
</commit_message>
<xml_diff>
--- a/weka-api-intro/excel z porownaniem.xlsx
+++ b/weka-api-intro/excel z porownaniem.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="75" windowWidth="20340" windowHeight="7950"/>
@@ -11,7 +11,7 @@
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -147,8 +147,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.8859857583527818E-2"/>
-          <c:y val="0.20861869743759506"/>
+          <c:x val="5.8859857583527811E-2"/>
+          <c:y val="0.20861869743759509"/>
           <c:w val="0.69853722326277934"/>
           <c:h val="0.66132778447739082"/>
         </c:manualLayout>
@@ -228,52 +228,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>22.458540175567901</c:v>
+                  <c:v>13.400848273903</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.221193492650698</c:v>
+                  <c:v>10.815406331455501</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.219848710345602</c:v>
+                  <c:v>8.3190737724788999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.131757600146699</c:v>
+                  <c:v>5.06442723116648</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>22.157061103723901</c:v>
+                  <c:v>5.3997836355662097</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.6292502921346</c:v>
+                  <c:v>4.2123322209833596</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.912717911471798</c:v>
+                  <c:v>3.8652110178089001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.649298760827101</c:v>
+                  <c:v>1.2505876130546001</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24.717832493657198</c:v>
+                  <c:v>1.0768884883729199</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24.567386046366899</c:v>
+                  <c:v>1.26645647860317</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>26.175118539667999</c:v>
+                  <c:v>0.53366731069754503</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>26.691529455675798</c:v>
+                  <c:v>0.41812359255477199</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27.3302105896434</c:v>
+                  <c:v>0.17438090185944</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>27.4258348103372</c:v>
+                  <c:v>0.17881364828808</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.665293049765101</c:v>
+                  <c:v>0.108316267855431</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>27.743968090753601</c:v>
+                  <c:v>0.14164426835451199</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -295,52 +295,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23.492954847959599</c:v>
+                  <c:v>1.4067243252424899</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -362,77 +362,77 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>50.506245890861202</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>49.27734375</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>51.345422116527899</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>51.7387543252594</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>52.031393819855303</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>52.093407319328797</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>51.597194175789099</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>51.756572626430298</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>51.472496164803701</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>54.041005291005199</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>54.5485510380622</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>54.532182398198501</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>54.768326758711297</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>55.209035812672099</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>55.7663673469388</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>55.649291453615803</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="62046976"/>
-        <c:axId val="65683840"/>
+        <c:axId val="81178624"/>
+        <c:axId val="81180160"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="62046976"/>
+        <c:axId val="81178624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65683840"/>
+        <c:crossAx val="81180160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="65683840"/>
+        <c:axId val="81180160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -440,7 +440,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="62046976"/>
+        <c:crossAx val="81178624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -453,7 +453,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -470,9 +470,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.8564304461942255E-2"/>
-          <c:y val="0.21002353579042057"/>
-          <c:w val="0.67025853018372705"/>
+          <c:x val="6.8564304461942269E-2"/>
+          <c:y val="0.21002353579042063"/>
+          <c:w val="0.67025853018372716"/>
           <c:h val="0.68831491134030798"/>
         </c:manualLayout>
       </c:layout>
@@ -794,25 +794,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="143027200"/>
-        <c:axId val="143181312"/>
+        <c:axId val="81186176"/>
+        <c:axId val="84878080"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="143027200"/>
+        <c:axId val="81186176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143181312"/>
+        <c:crossAx val="84878080"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="143181312"/>
+        <c:axId val="84878080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -820,7 +820,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="143027200"/>
+        <c:crossAx val="81186176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -834,7 +834,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -851,10 +851,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.8564304461942255E-2"/>
+          <c:x val="6.8564304461942269E-2"/>
           <c:y val="0.16620506943674293"/>
-          <c:w val="0.67025853018372705"/>
-          <c:h val="0.73213337769398557"/>
+          <c:w val="0.67025853018372716"/>
+          <c:h val="0.73213337769398579"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1232,25 +1232,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="87562496"/>
-        <c:axId val="87629824"/>
+        <c:axId val="84908288"/>
+        <c:axId val="83107840"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="87562496"/>
+        <c:axId val="84908288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87629824"/>
+        <c:crossAx val="83107840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="87629824"/>
+        <c:axId val="83107840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1258,7 +1258,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="87562496"/>
+        <c:crossAx val="84908288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1272,7 +1272,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1291,8 +1291,8 @@
           <c:yMode val="edge"/>
           <c:x val="6.8564304461942283E-2"/>
           <c:y val="0.16620506943674293"/>
-          <c:w val="0.67025853018372739"/>
-          <c:h val="0.7321333776939859"/>
+          <c:w val="0.67025853018372761"/>
+          <c:h val="0.73213337769398601"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1670,25 +1670,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="90157440"/>
-        <c:axId val="90158976"/>
+        <c:axId val="83133184"/>
+        <c:axId val="83134720"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="90157440"/>
+        <c:axId val="83133184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90158976"/>
+        <c:crossAx val="83134720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="90158976"/>
+        <c:axId val="83134720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1696,7 +1696,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="90157440"/>
+        <c:crossAx val="83133184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1710,7 +1710,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1727,8 +1727,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.8859857583527804E-2"/>
-          <c:y val="0.20861869743759512"/>
+          <c:x val="5.885985758352779E-2"/>
+          <c:y val="0.20861869743759517"/>
           <c:w val="0.69853722326277934"/>
           <c:h val="0.66132778447739082"/>
         </c:manualLayout>
@@ -1808,52 +1808,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>84.040169149598597</c:v>
+                  <c:v>34.230890183995697</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>82.062725788375502</c:v>
+                  <c:v>34.749907226827602</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>80.6980483202925</c:v>
+                  <c:v>36.760135303432698</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>81.846285194355403</c:v>
+                  <c:v>37.506514872319897</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>80.5414882722078</c:v>
+                  <c:v>37.812661566929599</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>80.419347406083403</c:v>
+                  <c:v>40.405845047425103</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>81.851882246602699</c:v>
+                  <c:v>42.378842294701499</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>82.001083646646705</c:v>
+                  <c:v>43.990451507974498</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>82.568191890236605</c:v>
+                  <c:v>45.127956419399297</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>82.296199476367505</c:v>
+                  <c:v>45.038722190116701</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>82.334849759754704</c:v>
+                  <c:v>45.519349376705101</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>82.511863412381501</c:v>
+                  <c:v>45.966862247424899</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>82.931051206173194</c:v>
+                  <c:v>45.783113619915902</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>83.199756441221695</c:v>
+                  <c:v>47.5472306908947</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>83.249091468584496</c:v>
+                  <c:v>46.936166891061703</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>83.819896914241795</c:v>
+                  <c:v>46.7947787421597</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1875,52 +1875,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>69.551966783522701</c:v>
+                  <c:v>28.879909218464299</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68.602994863489897</c:v>
+                  <c:v>28.724302397141301</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>69.167716011458495</c:v>
+                  <c:v>28.862859486133399</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>66.608924458810804</c:v>
+                  <c:v>28.538290257971301</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>65.3656024100314</c:v>
+                  <c:v>28.667954438285101</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>62.968807869957601</c:v>
+                  <c:v>28.509935146337899</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>62.246186669622702</c:v>
+                  <c:v>28.415603606310299</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>63.077187327418898</c:v>
+                  <c:v>28.4045696435834</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>63.187093764575998</c:v>
+                  <c:v>28.43620772617</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>63.284595570606697</c:v>
+                  <c:v>28.4682634821169</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>62.819609858059501</c:v>
+                  <c:v>28.464719261970799</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>63.373720586929501</c:v>
+                  <c:v>28.454134629011399</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>62.997780064170797</c:v>
+                  <c:v>28.404448646960699</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>62.158655962594203</c:v>
+                  <c:v>28.435974221518499</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>73.187662813205193</c:v>
+                  <c:v>26.458131399340299</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>69.856797880513597</c:v>
+                  <c:v>26.243528432396801</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1942,77 +1942,77 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>119.50667195138</c:v>
+                  <c:v>138.118055555555</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>119.802640603566</c:v>
+                  <c:v>132.875</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>119.871124260355</c:v>
+                  <c:v>124.375</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>120.03389023545699</c:v>
+                  <c:v>121.375</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>119.89769120251199</c:v>
+                  <c:v>115.31805555555501</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>119.952005259697</c:v>
+                  <c:v>110.79643990929701</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>119.940283293338</c:v>
+                  <c:v>104.79388888888801</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>120.05381558446101</c:v>
+                  <c:v>102.349444444444</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>120.013153065868</c:v>
+                  <c:v>101.153134920634</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>119.99353654242699</c:v>
+                  <c:v>98.038134920634903</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>120.07921788434901</c:v>
+                  <c:v>95.093134920634895</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>120.08893823629001</c:v>
+                  <c:v>94.072569503146397</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120.05769421323799</c:v>
+                  <c:v>93.844392006802707</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>120.14147222773001</c:v>
+                  <c:v>90.910222505668898</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>120.13918014665001</c:v>
+                  <c:v>86.903347505668904</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>120.22369246463199</c:v>
+                  <c:v>85.903347505668904</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="89929216"/>
-        <c:axId val="89930752"/>
+        <c:axId val="83151872"/>
+        <c:axId val="85205760"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="89929216"/>
+        <c:axId val="83151872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89930752"/>
+        <c:crossAx val="85205760"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89930752"/>
+        <c:axId val="85205760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2020,7 +2020,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="89929216"/>
+        <c:crossAx val="83151872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2033,7 +2033,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -2050,8 +2050,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.8859857583527783E-2"/>
-          <c:y val="0.20861869743759523"/>
+          <c:x val="5.8859857583527776E-2"/>
+          <c:y val="0.20861869743759526"/>
           <c:w val="0.69853722326277934"/>
           <c:h val="0.66132778447739082"/>
         </c:manualLayout>
@@ -2131,52 +2131,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>95.364992171624806</c:v>
+                  <c:v>47.823642521492999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>97.518059729301996</c:v>
+                  <c:v>54.416846984750798</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>96.042951862531098</c:v>
+                  <c:v>58.7525966896414</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>96.510346430549106</c:v>
+                  <c:v>60.431404772541697</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>95.871749133608503</c:v>
+                  <c:v>57.413816659517799</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>95.922101711986301</c:v>
+                  <c:v>58.209319894160501</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>96.074962786921503</c:v>
+                  <c:v>57.286621080828702</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>96.399586580942994</c:v>
+                  <c:v>55.499723993276</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>97.441942575547301</c:v>
+                  <c:v>53.8128933325833</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>96.884267629135707</c:v>
+                  <c:v>54.280971669795797</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>96.766979818136505</c:v>
+                  <c:v>53.4978320281609</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>97.050706982093004</c:v>
+                  <c:v>52.880065992855101</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>97.399068426625206</c:v>
+                  <c:v>51.981517443046997</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>97.242804521037698</c:v>
+                  <c:v>52.061704648048703</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>97.748634284505698</c:v>
+                  <c:v>51.458262788674901</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>97.790631800318394</c:v>
+                  <c:v>51.574289161732999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2198,52 +2198,52 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>78.642130034416397</c:v>
+                  <c:v>40.280355720765101</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>57.171319669943898</c:v>
+                  <c:v>30.138725929568</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.064636986348802</c:v>
+                  <c:v>31.4980105878887</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58.675133509852799</c:v>
+                  <c:v>29.577965665937601</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>72.892275946103496</c:v>
+                  <c:v>27.044785153983799</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>73.169291612954595</c:v>
+                  <c:v>27.197190337947699</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>62.174392832092103</c:v>
+                  <c:v>26.508462747839999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>72.163820690618195</c:v>
+                  <c:v>27.565599079246201</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>71.197319000236902</c:v>
+                  <c:v>27.103919021301799</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>75.290704311026701</c:v>
+                  <c:v>26.1490402324267</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>79.076445213970104</c:v>
+                  <c:v>26.416114184604002</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>77.769800904681503</c:v>
+                  <c:v>26.135486649297199</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>76.289297483427404</c:v>
+                  <c:v>26.0903434629728</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>79.484462421522593</c:v>
+                  <c:v>24.575412338229199</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>79.663426475513205</c:v>
+                  <c:v>24.412990590032301</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>77.770373495258795</c:v>
+                  <c:v>24.007296812517101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2265,77 +2265,77 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>121.49873203719299</c:v>
+                  <c:v>204</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>121.273084025854</c:v>
+                  <c:v>191.76</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>121.220683041184</c:v>
+                  <c:v>174.01</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>121.000742187499</c:v>
+                  <c:v>157.777777777777</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>120.997013944877</c:v>
+                  <c:v>152.0625</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>120.85010368555</c:v>
+                  <c:v>146.51</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>120.73154592780401</c:v>
+                  <c:v>133.76</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>120.77555744519999</c:v>
+                  <c:v>131.07944444444399</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>120.320158677685</c:v>
+                  <c:v>113.836097337006</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>120.369285167334</c:v>
+                  <c:v>108.406097337006</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>120.301142263759</c:v>
+                  <c:v>106.301930670339</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>120.322522309356</c:v>
+                  <c:v>106.246876417233</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>120.331348513984</c:v>
+                  <c:v>103.251971749251</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>120.354273504273</c:v>
+                  <c:v>101.2635430839</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>120.411634001488</c:v>
+                  <c:v>100.2635430839</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>120.44584315293299</c:v>
+                  <c:v>98.766944444444405</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="85249408"/>
-        <c:axId val="86493824"/>
+        <c:axId val="85218816"/>
+        <c:axId val="85220352"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85249408"/>
+        <c:axId val="85218816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="86493824"/>
+        <c:crossAx val="85220352"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="86493824"/>
+        <c:axId val="85220352"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2343,7 +2343,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85249408"/>
+        <c:crossAx val="85218816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2356,7 +2356,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -2369,14 +2369,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>704849</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>190499</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1247774</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2398,15 +2398,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2428,15 +2428,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>1133475</xdr:colOff>
-      <xdr:row>44</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>1057275</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2457,16 +2457,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>876300</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
-      <xdr:row>47</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2487,16 +2487,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1323975</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104776</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1228724</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>390526</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2517,16 +2517,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>485775</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>685799</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3325,8 +3325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="AD26" sqref="AD26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q55" sqref="Q55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3456,16 +3456,16 @@
         <v>0.2</v>
       </c>
       <c r="C4" s="2">
-        <v>32</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="E4" s="2">
         <v>0.77777777777777701</v>
       </c>
       <c r="F4" s="2">
-        <v>22.458540175567901</v>
+        <v>13.400848273903</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="2"/>
@@ -3473,16 +3473,16 @@
         <v>0.2</v>
       </c>
       <c r="J4" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" s="2">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="L4" s="2">
         <v>0.82110091743119196</v>
       </c>
       <c r="M4" s="2">
-        <v>84.040169149598597</v>
+        <v>34.230890183995697</v>
       </c>
       <c r="N4" s="8"/>
       <c r="O4" s="2"/>
@@ -3499,7 +3499,7 @@
         <v>0.76190476190476097</v>
       </c>
       <c r="T4" s="2">
-        <v>95.364992171624806</v>
+        <v>47.823642521492999</v>
       </c>
     </row>
     <row r="5" spans="1:20" ht="15">
@@ -3511,13 +3511,13 @@
         <v>0</v>
       </c>
       <c r="D5" s="2">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2">
         <v>0.82828282828282795</v>
       </c>
       <c r="F5" s="2">
-        <v>22.221193492650698</v>
+        <v>10.815406331455501</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="2"/>
@@ -3528,13 +3528,13 @@
         <v>0</v>
       </c>
       <c r="K5" s="2">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="L5" s="2">
         <v>0.81192660550458695</v>
       </c>
       <c r="M5" s="2">
-        <v>82.062725788375502</v>
+        <v>34.749907226827602</v>
       </c>
       <c r="N5" s="8"/>
       <c r="O5" s="2"/>
@@ -3545,13 +3545,13 @@
         <v>0</v>
       </c>
       <c r="R5" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S5" s="2">
         <v>0.72727272727272696</v>
       </c>
       <c r="T5" s="2">
-        <v>97.518059729301996</v>
+        <v>54.416846984750798</v>
       </c>
     </row>
     <row r="6" spans="1:20" ht="15">
@@ -3563,13 +3563,13 @@
         <v>0</v>
       </c>
       <c r="D6" s="2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="E6" s="2">
         <v>0.89898989898989901</v>
       </c>
       <c r="F6" s="2">
-        <v>21.219848710345602</v>
+        <v>8.3190737724788999</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="2"/>
@@ -3577,16 +3577,16 @@
         <v>0.3</v>
       </c>
       <c r="J6" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L6" s="2">
         <v>0.78899082568807299</v>
       </c>
       <c r="M6" s="2">
-        <v>80.6980483202925</v>
+        <v>36.760135303432698</v>
       </c>
       <c r="N6" s="8"/>
       <c r="O6" s="2"/>
@@ -3594,16 +3594,16 @@
         <v>0.3</v>
       </c>
       <c r="Q6" s="2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R6" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S6" s="2">
         <v>0.69696969696969702</v>
       </c>
       <c r="T6" s="2">
-        <v>96.042951862531098</v>
+        <v>58.7525966896414</v>
       </c>
     </row>
     <row r="7" spans="1:20" ht="15">
@@ -3612,16 +3612,16 @@
         <v>0.35</v>
       </c>
       <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2">
         <v>15</v>
-      </c>
-      <c r="D7" s="2">
-        <v>16</v>
       </c>
       <c r="E7" s="2">
         <v>0.92929292929292895</v>
       </c>
       <c r="F7" s="2">
-        <v>21.131757600146699</v>
+        <v>5.06442723116648</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="2"/>
@@ -3629,16 +3629,16 @@
         <v>0.35</v>
       </c>
       <c r="J7" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L7" s="2">
         <v>0.78899082568807299</v>
       </c>
       <c r="M7" s="2">
-        <v>81.846285194355403</v>
+        <v>37.506514872319897</v>
       </c>
       <c r="N7" s="8"/>
       <c r="O7" s="2"/>
@@ -3649,13 +3649,13 @@
         <v>0</v>
       </c>
       <c r="R7" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="S7" s="2">
         <v>0.68831168831168799</v>
       </c>
       <c r="T7" s="2">
-        <v>96.510346430549106</v>
+        <v>60.431404772541697</v>
       </c>
     </row>
     <row r="8" spans="1:20" ht="15">
@@ -3667,13 +3667,13 @@
         <v>0</v>
       </c>
       <c r="D8" s="2">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E8" s="2">
         <v>0.92929292929292895</v>
       </c>
       <c r="F8" s="2">
-        <v>22.157061103723901</v>
+        <v>5.3997836355662097</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="2"/>
@@ -3681,16 +3681,16 @@
         <v>0.39999999999999902</v>
       </c>
       <c r="J8" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K8" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L8" s="2">
         <v>0.78440366972477005</v>
       </c>
       <c r="M8" s="2">
-        <v>80.5414882722078</v>
+        <v>37.812661566929599</v>
       </c>
       <c r="N8" s="8"/>
       <c r="O8" s="2"/>
@@ -3701,13 +3701,13 @@
         <v>0</v>
       </c>
       <c r="R8" s="2">
-        <v>4</v>
+        <v>172</v>
       </c>
       <c r="S8" s="2">
         <v>0.722943722943722</v>
       </c>
       <c r="T8" s="2">
-        <v>95.871749133608503</v>
+        <v>57.413816659517799</v>
       </c>
     </row>
     <row r="9" spans="1:20" ht="15">
@@ -3716,7 +3716,7 @@
         <v>0.44999999999999901</v>
       </c>
       <c r="C9" s="2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2">
         <v>0</v>
@@ -3725,7 +3725,7 @@
         <v>0.94949494949494895</v>
       </c>
       <c r="F9" s="2">
-        <v>23.6292502921346</v>
+        <v>4.2123322209833596</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="2"/>
@@ -3733,16 +3733,16 @@
         <v>0.44999999999999901</v>
       </c>
       <c r="J9" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L9" s="2">
         <v>0.77522935779816504</v>
       </c>
       <c r="M9" s="2">
-        <v>80.419347406083403</v>
+        <v>40.405845047425103</v>
       </c>
       <c r="N9" s="8"/>
       <c r="O9" s="2"/>
@@ -3759,7 +3759,7 @@
         <v>0.722943722943722</v>
       </c>
       <c r="T9" s="2">
-        <v>95.922101711986301</v>
+        <v>58.209319894160501</v>
       </c>
     </row>
     <row r="10" spans="1:20" ht="15">
@@ -3777,7 +3777,7 @@
         <v>0.94949494949494895</v>
       </c>
       <c r="F10" s="2">
-        <v>23.912717911471798</v>
+        <v>3.8652110178089001</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="2"/>
@@ -3788,13 +3788,13 @@
         <v>0</v>
       </c>
       <c r="K10" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="L10" s="2">
         <v>0.74311926605504497</v>
       </c>
       <c r="M10" s="2">
-        <v>81.851882246602699</v>
+        <v>42.378842294701499</v>
       </c>
       <c r="N10" s="8"/>
       <c r="O10" s="2"/>
@@ -3802,16 +3802,16 @@
         <v>0.499999999999999</v>
       </c>
       <c r="Q10" s="2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="R10" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S10" s="2">
         <v>0.722943722943722</v>
       </c>
       <c r="T10" s="2">
-        <v>96.074962786921503</v>
+        <v>57.286621080828702</v>
       </c>
     </row>
     <row r="11" spans="1:20" ht="15">
@@ -3823,13 +3823,13 @@
         <v>0</v>
       </c>
       <c r="D11" s="2">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E11" s="2">
         <v>0.98989898989898994</v>
       </c>
       <c r="F11" s="2">
-        <v>24.649298760827101</v>
+        <v>1.2505876130546001</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="2"/>
@@ -3837,16 +3837,16 @@
         <v>0.54999999999999905</v>
       </c>
       <c r="J11" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L11" s="2">
         <v>0.75229357798165097</v>
       </c>
       <c r="M11" s="2">
-        <v>82.001083646646705</v>
+        <v>43.990451507974498</v>
       </c>
       <c r="N11" s="8"/>
       <c r="O11" s="2"/>
@@ -3857,13 +3857,13 @@
         <v>0</v>
       </c>
       <c r="R11" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S11" s="2">
         <v>0.73160173160173103</v>
       </c>
       <c r="T11" s="2">
-        <v>96.399586580942994</v>
+        <v>55.499723993276</v>
       </c>
     </row>
     <row r="12" spans="1:20" ht="15">
@@ -3881,7 +3881,7 @@
         <v>0.98989898989898994</v>
       </c>
       <c r="F12" s="2">
-        <v>24.717832493657198</v>
+        <v>1.0768884883729199</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="2"/>
@@ -3889,16 +3889,16 @@
         <v>0.6</v>
       </c>
       <c r="J12" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K12" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L12" s="2">
         <v>0.75688073394495403</v>
       </c>
       <c r="M12" s="2">
-        <v>82.568191890236605</v>
+        <v>45.127956419399297</v>
       </c>
       <c r="N12" s="8"/>
       <c r="O12" s="2"/>
@@ -3915,7 +3915,7 @@
         <v>0.73160173160173103</v>
       </c>
       <c r="T12" s="2">
-        <v>97.441942575547301</v>
+        <v>53.8128933325833</v>
       </c>
     </row>
     <row r="13" spans="1:20" ht="15">
@@ -3933,7 +3933,7 @@
         <v>0.98989898989898994</v>
       </c>
       <c r="F13" s="2">
-        <v>24.567386046366899</v>
+        <v>1.26645647860317</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="2"/>
@@ -3941,16 +3941,16 @@
         <v>0.65</v>
       </c>
       <c r="J13" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K13" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L13" s="2">
         <v>0.75688073394495403</v>
       </c>
       <c r="M13" s="2">
-        <v>82.296199476367505</v>
+        <v>45.038722190116701</v>
       </c>
       <c r="N13" s="8"/>
       <c r="O13" s="2"/>
@@ -3967,7 +3967,7 @@
         <v>0.73160173160173103</v>
       </c>
       <c r="T13" s="2">
-        <v>96.884267629135707</v>
+        <v>54.280971669795797</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="15">
@@ -3985,7 +3985,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="2">
-        <v>26.175118539667999</v>
+        <v>0.53366731069754503</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="2"/>
@@ -3996,13 +3996,13 @@
         <v>0</v>
       </c>
       <c r="K14" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L14" s="2">
         <v>0.74311926605504497</v>
       </c>
       <c r="M14" s="2">
-        <v>82.334849759754704</v>
+        <v>45.519349376705101</v>
       </c>
       <c r="N14" s="8"/>
       <c r="O14" s="2"/>
@@ -4013,13 +4013,13 @@
         <v>0</v>
       </c>
       <c r="R14" s="2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="S14" s="2">
         <v>0.74025974025973995</v>
       </c>
       <c r="T14" s="2">
-        <v>96.766979818136505</v>
+        <v>53.4978320281609</v>
       </c>
     </row>
     <row r="15" spans="1:20" ht="15">
@@ -4028,7 +4028,7 @@
         <v>0.75</v>
       </c>
       <c r="C15" s="2">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="D15" s="2">
         <v>0</v>
@@ -4037,7 +4037,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="2">
-        <v>26.691529455675798</v>
+        <v>0.41812359255477199</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="2"/>
@@ -4045,16 +4045,16 @@
         <v>0.75</v>
       </c>
       <c r="J15" s="2">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="K15" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L15" s="2">
         <v>0.75229357798165097</v>
       </c>
       <c r="M15" s="2">
-        <v>82.511863412381501</v>
+        <v>45.966862247424899</v>
       </c>
       <c r="N15" s="8"/>
       <c r="O15" s="2"/>
@@ -4071,7 +4071,7 @@
         <v>0.74891774891774798</v>
       </c>
       <c r="T15" s="2">
-        <v>97.050706982093004</v>
+        <v>52.880065992855101</v>
       </c>
     </row>
     <row r="16" spans="1:20" ht="15">
@@ -4089,7 +4089,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="2">
-        <v>27.3302105896434</v>
+        <v>0.17438090185944</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="2"/>
@@ -4097,16 +4097,16 @@
         <v>0.8</v>
       </c>
       <c r="J16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L16" s="2">
         <v>0.75229357798165097</v>
       </c>
       <c r="M16" s="2">
-        <v>82.931051206173194</v>
+        <v>45.783113619915902</v>
       </c>
       <c r="N16" s="8"/>
       <c r="O16" s="2"/>
@@ -4123,7 +4123,7 @@
         <v>0.74025974025973995</v>
       </c>
       <c r="T16" s="2">
-        <v>97.399068426625206</v>
+        <v>51.981517443046997</v>
       </c>
     </row>
     <row r="17" spans="1:20" ht="15">
@@ -4141,7 +4141,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="2">
-        <v>27.4258348103372</v>
+        <v>0.17881364828808</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="2"/>
@@ -4152,13 +4152,13 @@
         <v>0</v>
       </c>
       <c r="K17" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L17" s="2">
         <v>0.73394495412843996</v>
       </c>
       <c r="M17" s="2">
-        <v>83.199756441221695</v>
+        <v>47.5472306908947</v>
       </c>
       <c r="N17" s="8"/>
       <c r="O17" s="2"/>
@@ -4169,13 +4169,13 @@
         <v>0</v>
       </c>
       <c r="R17" s="2">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="S17" s="2">
         <v>0.74891774891774798</v>
       </c>
       <c r="T17" s="2">
-        <v>97.242804521037698</v>
+        <v>52.061704648048703</v>
       </c>
     </row>
     <row r="18" spans="1:20" ht="15">
@@ -4187,13 +4187,13 @@
         <v>0</v>
       </c>
       <c r="D18" s="2">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E18" s="2">
         <v>1</v>
       </c>
       <c r="F18" s="2">
-        <v>27.665293049765101</v>
+        <v>0.108316267855431</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="2"/>
@@ -4201,16 +4201,16 @@
         <v>0.9</v>
       </c>
       <c r="J18" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" s="2">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="L18" s="2">
         <v>0.74311926605504497</v>
       </c>
       <c r="M18" s="2">
-        <v>83.249091468584496</v>
+        <v>46.936166891061703</v>
       </c>
       <c r="N18" s="8"/>
       <c r="O18" s="2"/>
@@ -4221,13 +4221,13 @@
         <v>0</v>
       </c>
       <c r="R18" s="2">
-        <v>245</v>
+        <v>0</v>
       </c>
       <c r="S18" s="2">
         <v>0.75757575757575701</v>
       </c>
       <c r="T18" s="2">
-        <v>97.748634284505698</v>
+        <v>51.458262788674901</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="15">
@@ -4245,7 +4245,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="2">
-        <v>27.743968090753601</v>
+        <v>0.14164426835451199</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="2"/>
@@ -4253,16 +4253,16 @@
         <v>0.95</v>
       </c>
       <c r="J19" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="L19" s="2">
         <v>0.73853211009174302</v>
       </c>
       <c r="M19" s="2">
-        <v>83.819896914241795</v>
+        <v>46.7947787421597</v>
       </c>
       <c r="N19" s="8"/>
       <c r="O19" s="2"/>
@@ -4279,7 +4279,7 @@
         <v>0.75324675324675305</v>
       </c>
       <c r="T19" s="2">
-        <v>97.790631800318394</v>
+        <v>51.574289161732999</v>
       </c>
     </row>
     <row r="20" spans="1:20" ht="15">
@@ -4316,16 +4316,16 @@
         <v>0.2</v>
       </c>
       <c r="C21" s="3">
-        <v>319</v>
+        <v>187</v>
       </c>
       <c r="D21" s="3">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E21" s="3">
         <v>1</v>
       </c>
       <c r="F21" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="3"/>
@@ -4333,16 +4333,16 @@
         <v>0.2</v>
       </c>
       <c r="J21" s="3">
-        <v>78</v>
+        <v>47</v>
       </c>
       <c r="K21" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L21" s="3">
         <v>0.83944954128440297</v>
       </c>
       <c r="M21" s="3">
-        <v>69.551966783522701</v>
+        <v>28.879909218464299</v>
       </c>
       <c r="N21" s="8"/>
       <c r="O21" s="3"/>
@@ -4350,7 +4350,7 @@
         <v>0.2</v>
       </c>
       <c r="Q21" s="3">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="R21" s="3">
         <v>0</v>
@@ -4359,7 +4359,7 @@
         <v>0.74891774891774798</v>
       </c>
       <c r="T21" s="3">
-        <v>78.642130034416397</v>
+        <v>40.280355720765101</v>
       </c>
     </row>
     <row r="22" spans="1:20" ht="15">
@@ -4368,16 +4368,16 @@
         <v>0.25</v>
       </c>
       <c r="C22" s="3">
-        <v>125</v>
+        <v>46</v>
       </c>
       <c r="D22" s="3">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E22" s="3">
         <v>1</v>
       </c>
       <c r="F22" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G22" s="8"/>
       <c r="H22" s="3"/>
@@ -4385,7 +4385,7 @@
         <v>0.25</v>
       </c>
       <c r="J22" s="3">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="K22" s="3">
         <v>0</v>
@@ -4394,7 +4394,7 @@
         <v>0.83944954128440297</v>
       </c>
       <c r="M22" s="3">
-        <v>68.602994863489897</v>
+        <v>28.724302397141301</v>
       </c>
       <c r="N22" s="8"/>
       <c r="O22" s="3"/>
@@ -4402,16 +4402,16 @@
         <v>0.25</v>
       </c>
       <c r="Q22" s="3">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="R22" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S22" s="3">
         <v>0.86147186147186094</v>
       </c>
       <c r="T22" s="3">
-        <v>57.171319669943898</v>
+        <v>30.138725929568</v>
       </c>
     </row>
     <row r="23" spans="1:20" ht="15">
@@ -4420,16 +4420,16 @@
         <v>0.3</v>
       </c>
       <c r="C23" s="3">
-        <v>68</v>
+        <v>31</v>
       </c>
       <c r="D23" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E23" s="3">
         <v>1</v>
       </c>
       <c r="F23" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="3"/>
@@ -4437,16 +4437,16 @@
         <v>0.3</v>
       </c>
       <c r="J23" s="3">
-        <v>126</v>
+        <v>62</v>
       </c>
       <c r="K23" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L23" s="3">
         <v>0.83944954128440297</v>
       </c>
       <c r="M23" s="3">
-        <v>69.167716011458495</v>
+        <v>28.862859486133399</v>
       </c>
       <c r="N23" s="8"/>
       <c r="O23" s="3"/>
@@ -4454,16 +4454,16 @@
         <v>0.3</v>
       </c>
       <c r="Q23" s="3">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="R23" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="S23" s="3">
         <v>0.80952380952380898</v>
       </c>
       <c r="T23" s="3">
-        <v>71.064636986348802</v>
+        <v>31.4980105878887</v>
       </c>
     </row>
     <row r="24" spans="1:20" ht="15">
@@ -4472,16 +4472,16 @@
         <v>0.35</v>
       </c>
       <c r="C24" s="3">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="D24" s="3">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E24" s="3">
         <v>1</v>
       </c>
       <c r="F24" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G24" s="8"/>
       <c r="H24" s="3"/>
@@ -4489,16 +4489,16 @@
         <v>0.35</v>
       </c>
       <c r="J24" s="3">
-        <v>132</v>
+        <v>78</v>
       </c>
       <c r="K24" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L24" s="3">
         <v>0.83944954128440297</v>
       </c>
       <c r="M24" s="3">
-        <v>66.608924458810804</v>
+        <v>28.538290257971301</v>
       </c>
       <c r="N24" s="8"/>
       <c r="O24" s="3"/>
@@ -4506,7 +4506,7 @@
         <v>0.35</v>
       </c>
       <c r="Q24" s="3">
-        <v>117</v>
+        <v>78</v>
       </c>
       <c r="R24" s="3">
         <v>0</v>
@@ -4515,7 +4515,7 @@
         <v>0.86147186147186094</v>
       </c>
       <c r="T24" s="3">
-        <v>58.675133509852799</v>
+        <v>29.577965665937601</v>
       </c>
     </row>
     <row r="25" spans="1:20" ht="15">
@@ -4524,16 +4524,16 @@
         <v>0.39999999999999902</v>
       </c>
       <c r="C25" s="3">
-        <v>47</v>
+        <v>16</v>
       </c>
       <c r="D25" s="3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E25" s="3">
         <v>1</v>
       </c>
       <c r="F25" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G25" s="8"/>
       <c r="H25" s="3"/>
@@ -4541,16 +4541,16 @@
         <v>0.39999999999999902</v>
       </c>
       <c r="J25" s="3">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="K25" s="3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L25" s="3">
         <v>0.83944954128440297</v>
       </c>
       <c r="M25" s="3">
-        <v>65.3656024100314</v>
+        <v>28.667954438285101</v>
       </c>
       <c r="N25" s="8"/>
       <c r="O25" s="3"/>
@@ -4558,7 +4558,7 @@
         <v>0.39999999999999902</v>
       </c>
       <c r="Q25" s="3">
-        <v>128</v>
+        <v>78</v>
       </c>
       <c r="R25" s="3">
         <v>0</v>
@@ -4567,7 +4567,7 @@
         <v>0.82683982683982604</v>
       </c>
       <c r="T25" s="3">
-        <v>72.892275946103496</v>
+        <v>27.044785153983799</v>
       </c>
     </row>
     <row r="26" spans="1:20" ht="15">
@@ -4576,16 +4576,16 @@
         <v>0.44999999999999901</v>
       </c>
       <c r="C26" s="3">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D26" s="3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E26" s="3">
         <v>1</v>
       </c>
       <c r="F26" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="3"/>
@@ -4593,7 +4593,7 @@
         <v>0.44999999999999901</v>
       </c>
       <c r="J26" s="3">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="K26" s="3">
         <v>0</v>
@@ -4602,7 +4602,7 @@
         <v>0.83944954128440297</v>
       </c>
       <c r="M26" s="3">
-        <v>62.968807869957601</v>
+        <v>28.509935146337899</v>
       </c>
       <c r="N26" s="8"/>
       <c r="O26" s="3"/>
@@ -4610,16 +4610,16 @@
         <v>0.44999999999999901</v>
       </c>
       <c r="Q26" s="3">
-        <v>183</v>
+        <v>94</v>
       </c>
       <c r="R26" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S26" s="3">
         <v>0.85714285714285698</v>
       </c>
       <c r="T26" s="3">
-        <v>73.169291612954595</v>
+        <v>27.197190337947699</v>
       </c>
     </row>
     <row r="27" spans="1:20" ht="15">
@@ -4631,13 +4631,13 @@
         <v>31</v>
       </c>
       <c r="D27" s="3">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="E27" s="3">
         <v>1</v>
       </c>
       <c r="F27" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G27" s="8"/>
       <c r="H27" s="3"/>
@@ -4645,16 +4645,16 @@
         <v>0.499999999999999</v>
       </c>
       <c r="J27" s="3">
-        <v>141</v>
+        <v>110</v>
       </c>
       <c r="K27" s="3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="L27" s="3">
         <v>0.83944954128440297</v>
       </c>
       <c r="M27" s="3">
-        <v>62.246186669622702</v>
+        <v>28.415603606310299</v>
       </c>
       <c r="N27" s="8"/>
       <c r="O27" s="3"/>
@@ -4662,7 +4662,7 @@
         <v>0.499999999999999</v>
       </c>
       <c r="Q27" s="3">
-        <v>146</v>
+        <v>94</v>
       </c>
       <c r="R27" s="3">
         <v>0</v>
@@ -4671,7 +4671,7 @@
         <v>0.87012987012986998</v>
       </c>
       <c r="T27" s="3">
-        <v>62.174392832092103</v>
+        <v>26.508462747839999</v>
       </c>
     </row>
     <row r="28" spans="1:20" ht="15">
@@ -4680,7 +4680,7 @@
         <v>0.54999999999999905</v>
       </c>
       <c r="C28" s="3">
-        <v>62</v>
+        <v>31</v>
       </c>
       <c r="D28" s="3">
         <v>0</v>
@@ -4689,7 +4689,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G28" s="8"/>
       <c r="H28" s="3"/>
@@ -4697,16 +4697,16 @@
         <v>0.54999999999999905</v>
       </c>
       <c r="J28" s="3">
-        <v>176</v>
+        <v>124</v>
       </c>
       <c r="K28" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L28" s="3">
         <v>0.83944954128440297</v>
       </c>
       <c r="M28" s="3">
-        <v>63.077187327418898</v>
+        <v>28.4045696435834</v>
       </c>
       <c r="N28" s="8"/>
       <c r="O28" s="3"/>
@@ -4714,7 +4714,7 @@
         <v>0.54999999999999905</v>
       </c>
       <c r="Q28" s="3">
-        <v>163</v>
+        <v>93</v>
       </c>
       <c r="R28" s="3">
         <v>0</v>
@@ -4723,7 +4723,7 @@
         <v>0.80952380952380898</v>
       </c>
       <c r="T28" s="3">
-        <v>72.163820690618195</v>
+        <v>27.565599079246201</v>
       </c>
     </row>
     <row r="29" spans="1:20" ht="15">
@@ -4732,7 +4732,7 @@
         <v>0.6</v>
       </c>
       <c r="C29" s="3">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D29" s="3">
         <v>0</v>
@@ -4741,7 +4741,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G29" s="8"/>
       <c r="H29" s="3"/>
@@ -4749,7 +4749,7 @@
         <v>0.6</v>
       </c>
       <c r="J29" s="3">
-        <v>157</v>
+        <v>110</v>
       </c>
       <c r="K29" s="3">
         <v>0</v>
@@ -4758,7 +4758,7 @@
         <v>0.83944954128440297</v>
       </c>
       <c r="M29" s="3">
-        <v>63.187093764575998</v>
+        <v>28.43620772617</v>
       </c>
       <c r="N29" s="8"/>
       <c r="O29" s="3"/>
@@ -4766,7 +4766,7 @@
         <v>0.6</v>
       </c>
       <c r="Q29" s="3">
-        <v>212</v>
+        <v>125</v>
       </c>
       <c r="R29" s="3">
         <v>0</v>
@@ -4775,7 +4775,7 @@
         <v>0.831168831168831</v>
       </c>
       <c r="T29" s="3">
-        <v>71.197319000236902</v>
+        <v>27.103919021301799</v>
       </c>
     </row>
     <row r="30" spans="1:20" ht="15">
@@ -4784,16 +4784,16 @@
         <v>0.65</v>
       </c>
       <c r="C30" s="3">
-        <v>59</v>
+        <v>31</v>
       </c>
       <c r="D30" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="3">
         <v>1</v>
       </c>
       <c r="F30" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G30" s="8"/>
       <c r="H30" s="3"/>
@@ -4801,16 +4801,16 @@
         <v>0.65</v>
       </c>
       <c r="J30" s="3">
-        <v>187</v>
+        <v>126</v>
       </c>
       <c r="K30" s="3">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="L30" s="3">
         <v>0.83944954128440297</v>
       </c>
       <c r="M30" s="3">
-        <v>63.284595570606697</v>
+        <v>28.4682634821169</v>
       </c>
       <c r="N30" s="8"/>
       <c r="O30" s="3"/>
@@ -4818,7 +4818,7 @@
         <v>0.65</v>
       </c>
       <c r="Q30" s="3">
-        <v>366</v>
+        <v>172</v>
       </c>
       <c r="R30" s="3">
         <v>0</v>
@@ -4827,7 +4827,7 @@
         <v>0.84415584415584399</v>
       </c>
       <c r="T30" s="3">
-        <v>75.290704311026701</v>
+        <v>26.1490402324267</v>
       </c>
     </row>
     <row r="31" spans="1:20" ht="15">
@@ -4836,7 +4836,7 @@
         <v>0.7</v>
       </c>
       <c r="C31" s="3">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D31" s="3">
         <v>0</v>
@@ -4845,7 +4845,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="3"/>
@@ -4853,7 +4853,7 @@
         <v>0.7</v>
       </c>
       <c r="J31" s="3">
-        <v>259</v>
+        <v>187</v>
       </c>
       <c r="K31" s="3">
         <v>0</v>
@@ -4862,7 +4862,7 @@
         <v>0.83944954128440297</v>
       </c>
       <c r="M31" s="3">
-        <v>62.819609858059501</v>
+        <v>28.464719261970799</v>
       </c>
       <c r="N31" s="8"/>
       <c r="O31" s="3"/>
@@ -4870,16 +4870,16 @@
         <v>0.7</v>
       </c>
       <c r="Q31" s="3">
-        <v>338</v>
+        <v>187</v>
       </c>
       <c r="R31" s="3">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="S31" s="3">
         <v>0.83549783549783496</v>
       </c>
       <c r="T31" s="3">
-        <v>79.076445213970104</v>
+        <v>26.416114184604002</v>
       </c>
     </row>
     <row r="32" spans="1:20" ht="15">
@@ -4888,7 +4888,7 @@
         <v>0.75</v>
       </c>
       <c r="C32" s="3">
-        <v>63</v>
+        <v>31</v>
       </c>
       <c r="D32" s="3">
         <v>0</v>
@@ -4897,7 +4897,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G32" s="8"/>
       <c r="H32" s="3"/>
@@ -4905,7 +4905,7 @@
         <v>0.75</v>
       </c>
       <c r="J32" s="3">
-        <v>212</v>
+        <v>125</v>
       </c>
       <c r="K32" s="3">
         <v>0</v>
@@ -4914,7 +4914,7 @@
         <v>0.83944954128440297</v>
       </c>
       <c r="M32" s="3">
-        <v>63.373720586929501</v>
+        <v>28.454134629011399</v>
       </c>
       <c r="N32" s="8"/>
       <c r="O32" s="3"/>
@@ -4922,16 +4922,16 @@
         <v>0.75</v>
       </c>
       <c r="Q32" s="3">
-        <v>334</v>
+        <v>203</v>
       </c>
       <c r="R32" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S32" s="3">
         <v>0.831168831168831</v>
       </c>
       <c r="T32" s="3">
-        <v>77.769800904681503</v>
+        <v>26.135486649297199</v>
       </c>
     </row>
     <row r="33" spans="1:20" ht="15">
@@ -4940,16 +4940,16 @@
         <v>0.8</v>
       </c>
       <c r="C33" s="3">
-        <v>75</v>
+        <v>47</v>
       </c>
       <c r="D33" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E33" s="3">
         <v>1</v>
       </c>
       <c r="F33" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G33" s="8"/>
       <c r="H33" s="3"/>
@@ -4957,16 +4957,16 @@
         <v>0.8</v>
       </c>
       <c r="J33" s="3">
-        <v>221</v>
+        <v>156</v>
       </c>
       <c r="K33" s="3">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="L33" s="3">
         <v>0.83944954128440297</v>
       </c>
       <c r="M33" s="3">
-        <v>62.997780064170797</v>
+        <v>28.404448646960699</v>
       </c>
       <c r="N33" s="8"/>
       <c r="O33" s="3"/>
@@ -4974,16 +4974,16 @@
         <v>0.8</v>
       </c>
       <c r="Q33" s="3">
-        <v>343</v>
+        <v>218</v>
       </c>
       <c r="R33" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S33" s="3">
         <v>0.84848484848484795</v>
       </c>
       <c r="T33" s="3">
-        <v>76.289297483427404</v>
+        <v>26.0903434629728</v>
       </c>
     </row>
     <row r="34" spans="1:20" ht="15">
@@ -4992,16 +4992,16 @@
         <v>0.85</v>
       </c>
       <c r="C34" s="3">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="D34" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E34" s="3">
         <v>1</v>
       </c>
       <c r="F34" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G34" s="8"/>
       <c r="H34" s="3"/>
@@ -5009,16 +5009,16 @@
         <v>0.85</v>
       </c>
       <c r="J34" s="3">
-        <v>234</v>
+        <v>172</v>
       </c>
       <c r="K34" s="3">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="L34" s="3">
         <v>0.83944954128440297</v>
       </c>
       <c r="M34" s="3">
-        <v>62.158655962594203</v>
+        <v>28.435974221518499</v>
       </c>
       <c r="N34" s="8"/>
       <c r="O34" s="3"/>
@@ -5026,7 +5026,7 @@
         <v>0.85</v>
       </c>
       <c r="Q34" s="3">
-        <v>249</v>
+        <v>173</v>
       </c>
       <c r="R34" s="3">
         <v>0</v>
@@ -5035,7 +5035,7 @@
         <v>0.85714285714285698</v>
       </c>
       <c r="T34" s="3">
-        <v>79.484462421522593</v>
+        <v>24.575412338229199</v>
       </c>
     </row>
     <row r="35" spans="1:20" ht="15">
@@ -5044,16 +5044,16 @@
         <v>0.9</v>
       </c>
       <c r="C35" s="3">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D35" s="3">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E35" s="3">
         <v>1</v>
       </c>
       <c r="F35" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G35" s="8"/>
       <c r="H35" s="3"/>
@@ -5061,7 +5061,7 @@
         <v>0.9</v>
       </c>
       <c r="J35" s="3">
-        <v>303</v>
+        <v>202</v>
       </c>
       <c r="K35" s="3">
         <v>0</v>
@@ -5070,7 +5070,7 @@
         <v>0.83944954128440297</v>
       </c>
       <c r="M35" s="3">
-        <v>73.187662813205193</v>
+        <v>26.458131399340299</v>
       </c>
       <c r="N35" s="8"/>
       <c r="O35" s="3"/>
@@ -5078,16 +5078,16 @@
         <v>0.9</v>
       </c>
       <c r="Q35" s="3">
-        <v>306</v>
+        <v>203</v>
       </c>
       <c r="R35" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="S35" s="3">
         <v>0.85281385281385202</v>
       </c>
       <c r="T35" s="3">
-        <v>79.663426475513205</v>
+        <v>24.412990590032301</v>
       </c>
     </row>
     <row r="36" spans="1:20" ht="15">
@@ -5096,16 +5096,16 @@
         <v>0.95</v>
       </c>
       <c r="C36" s="3">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="D36" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E36" s="3">
         <v>1</v>
       </c>
       <c r="F36" s="3">
-        <v>23.492954847959599</v>
+        <v>1.4067243252424899</v>
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="3"/>
@@ -5113,7 +5113,7 @@
         <v>0.95</v>
       </c>
       <c r="J36" s="3">
-        <v>410</v>
+        <v>266</v>
       </c>
       <c r="K36" s="3">
         <v>0</v>
@@ -5122,7 +5122,7 @@
         <v>0.83027522935779796</v>
       </c>
       <c r="M36" s="3">
-        <v>69.856797880513597</v>
+        <v>26.243528432396801</v>
       </c>
       <c r="N36" s="8"/>
       <c r="O36" s="3"/>
@@ -5130,16 +5130,16 @@
         <v>0.95</v>
       </c>
       <c r="Q36" s="3">
-        <v>371</v>
+        <v>219</v>
       </c>
       <c r="R36" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S36" s="3">
         <v>0.84415584415584399</v>
       </c>
       <c r="T36" s="3">
-        <v>77.770373495258795</v>
+        <v>24.007296812517101</v>
       </c>
     </row>
     <row r="37" spans="1:20" ht="15">
@@ -5176,16 +5176,16 @@
         <v>0.2</v>
       </c>
       <c r="C38" s="4">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D38" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E38" s="4">
         <v>0.86868686868686795</v>
       </c>
       <c r="F38" s="4">
-        <v>50.506245890861202</v>
+        <v>33</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="4"/>
@@ -5193,16 +5193,16 @@
         <v>0.2</v>
       </c>
       <c r="J38" s="4">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="K38" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="L38" s="4">
         <v>0.66513761467889898</v>
       </c>
       <c r="M38" s="4">
-        <v>119.50667195138</v>
+        <v>138.118055555555</v>
       </c>
       <c r="N38" s="8"/>
       <c r="O38" s="4"/>
@@ -5210,7 +5210,7 @@
         <v>0.2</v>
       </c>
       <c r="Q38" s="4">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="R38" s="4">
         <v>0</v>
@@ -5219,7 +5219,7 @@
         <v>0.53679653679653605</v>
       </c>
       <c r="T38" s="4">
-        <v>121.49873203719299</v>
+        <v>204</v>
       </c>
     </row>
     <row r="39" spans="1:20" ht="15">
@@ -5228,16 +5228,16 @@
         <v>0.25</v>
       </c>
       <c r="C39" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D39" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E39" s="4">
         <v>0.86868686868686795</v>
       </c>
       <c r="F39" s="4">
-        <v>49.27734375</v>
+        <v>33</v>
       </c>
       <c r="G39" s="8"/>
       <c r="H39" s="4"/>
@@ -5245,16 +5245,16 @@
         <v>0.25</v>
       </c>
       <c r="J39" s="4">
-        <v>32</v>
+        <v>0</v>
       </c>
       <c r="K39" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L39" s="4">
         <v>0.67431192660550399</v>
       </c>
       <c r="M39" s="4">
-        <v>119.802640603566</v>
+        <v>132.875</v>
       </c>
       <c r="N39" s="8"/>
       <c r="O39" s="4"/>
@@ -5262,7 +5262,7 @@
         <v>0.25</v>
       </c>
       <c r="Q39" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="R39" s="4">
         <v>0</v>
@@ -5271,7 +5271,7 @@
         <v>0.54545454545454497</v>
       </c>
       <c r="T39" s="4">
-        <v>121.273084025854</v>
+        <v>191.76</v>
       </c>
     </row>
     <row r="40" spans="1:20" ht="15">
@@ -5280,16 +5280,16 @@
         <v>0.3</v>
       </c>
       <c r="C40" s="4">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D40" s="4">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="E40" s="4">
         <v>0.90909090909090895</v>
       </c>
       <c r="F40" s="4">
-        <v>51.345422116527899</v>
+        <v>22</v>
       </c>
       <c r="G40" s="8"/>
       <c r="H40" s="4"/>
@@ -5297,16 +5297,16 @@
         <v>0.3</v>
       </c>
       <c r="J40" s="4">
-        <v>29</v>
+        <v>94</v>
       </c>
       <c r="K40" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L40" s="4">
         <v>0.67889908256880704</v>
       </c>
       <c r="M40" s="4">
-        <v>119.871124260355</v>
+        <v>124.375</v>
       </c>
       <c r="N40" s="8"/>
       <c r="O40" s="4"/>
@@ -5323,7 +5323,7 @@
         <v>0.58008658008657998</v>
       </c>
       <c r="T40" s="4">
-        <v>121.220683041184</v>
+        <v>174.01</v>
       </c>
     </row>
     <row r="41" spans="1:20" ht="15">
@@ -5332,16 +5332,16 @@
         <v>0.35</v>
       </c>
       <c r="C41" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D41" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E41" s="4">
         <v>0.90909090909090895</v>
       </c>
       <c r="F41" s="4">
-        <v>51.7387543252594</v>
+        <v>22</v>
       </c>
       <c r="G41" s="8"/>
       <c r="H41" s="4"/>
@@ -5349,16 +5349,16 @@
         <v>0.35</v>
       </c>
       <c r="J41" s="4">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="K41" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L41" s="4">
         <v>0.68348623853210999</v>
       </c>
       <c r="M41" s="4">
-        <v>120.03389023545699</v>
+        <v>121.375</v>
       </c>
       <c r="N41" s="8"/>
       <c r="O41" s="4"/>
@@ -5366,16 +5366,16 @@
         <v>0.35</v>
       </c>
       <c r="Q41" s="4">
-        <v>114</v>
+        <v>0</v>
       </c>
       <c r="R41" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S41" s="4">
         <v>0.59307359307359298</v>
       </c>
       <c r="T41" s="4">
-        <v>121.000742187499</v>
+        <v>157.777777777777</v>
       </c>
     </row>
     <row r="42" spans="1:20" ht="15">
@@ -5384,16 +5384,16 @@
         <v>0.39999999999999902</v>
       </c>
       <c r="C42" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D42" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E42" s="4">
         <v>0.90909090909090895</v>
       </c>
       <c r="F42" s="4">
-        <v>52.031393819855303</v>
+        <v>22</v>
       </c>
       <c r="G42" s="8"/>
       <c r="H42" s="4"/>
@@ -5401,16 +5401,16 @@
         <v>0.39999999999999902</v>
       </c>
       <c r="J42" s="4">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="K42" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L42" s="4">
         <v>0.68348623853210999</v>
       </c>
       <c r="M42" s="4">
-        <v>119.89769120251199</v>
+        <v>115.31805555555501</v>
       </c>
       <c r="N42" s="8"/>
       <c r="O42" s="4"/>
@@ -5418,7 +5418,7 @@
         <v>0.39999999999999902</v>
       </c>
       <c r="Q42" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="R42" s="4">
         <v>0</v>
@@ -5427,7 +5427,7 @@
         <v>0.61038961038961004</v>
       </c>
       <c r="T42" s="4">
-        <v>120.997013944877</v>
+        <v>152.0625</v>
       </c>
     </row>
     <row r="43" spans="1:20">
@@ -5436,16 +5436,16 @@
         <v>0.44999999999999901</v>
       </c>
       <c r="C43" s="4">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="D43" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E43" s="4">
         <v>0.90909090909090895</v>
       </c>
       <c r="F43" s="4">
-        <v>52.093407319328797</v>
+        <v>22</v>
       </c>
       <c r="G43" s="8"/>
       <c r="H43" s="4"/>
@@ -5453,16 +5453,16 @@
         <v>0.44999999999999901</v>
       </c>
       <c r="J43" s="4">
-        <v>26</v>
+        <v>140</v>
       </c>
       <c r="K43" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L43" s="4">
         <v>0.69724770642201805</v>
       </c>
       <c r="M43" s="4">
-        <v>119.952005259697</v>
+        <v>110.79643990929701</v>
       </c>
       <c r="N43" s="8"/>
       <c r="O43" s="4"/>
@@ -5479,7 +5479,7 @@
         <v>0.61904761904761896</v>
       </c>
       <c r="T43" s="4">
-        <v>120.85010368555</v>
+        <v>146.51</v>
       </c>
     </row>
     <row r="44" spans="1:20">
@@ -5488,16 +5488,16 @@
         <v>0.499999999999999</v>
       </c>
       <c r="C44" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D44" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E44" s="4">
         <v>0.90909090909090895</v>
       </c>
       <c r="F44" s="4">
-        <v>51.597194175789099</v>
+        <v>22</v>
       </c>
       <c r="G44" s="8"/>
       <c r="H44" s="4"/>
@@ -5505,16 +5505,16 @@
         <v>0.499999999999999</v>
       </c>
       <c r="J44" s="4">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="K44" s="4">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="L44" s="4">
         <v>0.71559633027522895</v>
       </c>
       <c r="M44" s="4">
-        <v>119.940283293338</v>
+        <v>104.79388888888801</v>
       </c>
       <c r="N44" s="8"/>
       <c r="O44" s="4"/>
@@ -5522,7 +5522,7 @@
         <v>0.499999999999999</v>
       </c>
       <c r="Q44" s="4">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="R44" s="4">
         <v>0</v>
@@ -5531,7 +5531,7 @@
         <v>0.65800865800865804</v>
       </c>
       <c r="T44" s="4">
-        <v>120.73154592780401</v>
+        <v>133.76</v>
       </c>
     </row>
     <row r="45" spans="1:20">
@@ -5540,16 +5540,16 @@
         <v>0.54999999999999905</v>
       </c>
       <c r="C45" s="4">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="D45" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E45" s="4">
         <v>0.90909090909090895</v>
       </c>
       <c r="F45" s="4">
-        <v>51.756572626430298</v>
+        <v>21</v>
       </c>
       <c r="G45" s="8"/>
       <c r="H45" s="4"/>
@@ -5557,16 +5557,16 @@
         <v>0.54999999999999905</v>
       </c>
       <c r="J45" s="4">
-        <v>104</v>
+        <v>0</v>
       </c>
       <c r="K45" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L45" s="4">
         <v>0.70642201834862295</v>
       </c>
       <c r="M45" s="4">
-        <v>120.05381558446101</v>
+        <v>102.349444444444</v>
       </c>
       <c r="N45" s="8"/>
       <c r="O45" s="4"/>
@@ -5574,7 +5574,7 @@
         <v>0.54999999999999905</v>
       </c>
       <c r="Q45" s="4">
-        <v>15</v>
+        <v>0</v>
       </c>
       <c r="R45" s="4">
         <v>0</v>
@@ -5583,7 +5583,7 @@
         <v>0.66666666666666596</v>
       </c>
       <c r="T45" s="4">
-        <v>120.77555744519999</v>
+        <v>131.07944444444399</v>
       </c>
     </row>
     <row r="46" spans="1:20">
@@ -5592,16 +5592,16 @@
         <v>0.6</v>
       </c>
       <c r="C46" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E46" s="4">
         <v>0.90909090909090895</v>
       </c>
       <c r="F46" s="4">
-        <v>51.472496164803701</v>
+        <v>21</v>
       </c>
       <c r="G46" s="8"/>
       <c r="H46" s="4"/>
@@ -5609,16 +5609,16 @@
         <v>0.6</v>
       </c>
       <c r="J46" s="4">
-        <v>252</v>
+        <v>140</v>
       </c>
       <c r="K46" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="L46" s="4">
         <v>0.71100917431192601</v>
       </c>
       <c r="M46" s="4">
-        <v>120.013153065868</v>
+        <v>101.153134920634</v>
       </c>
       <c r="N46" s="8"/>
       <c r="O46" s="4"/>
@@ -5626,16 +5626,16 @@
         <v>0.6</v>
       </c>
       <c r="Q46" s="4">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="R46" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S46" s="4">
         <v>0.71428571428571397</v>
       </c>
       <c r="T46" s="4">
-        <v>120.320158677685</v>
+        <v>113.836097337006</v>
       </c>
     </row>
     <row r="47" spans="1:20">
@@ -5644,7 +5644,7 @@
         <v>0.65</v>
       </c>
       <c r="C47" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D47" s="4">
         <v>0</v>
@@ -5653,7 +5653,7 @@
         <v>0.94949494949494895</v>
       </c>
       <c r="F47" s="4">
-        <v>54.041005291005199</v>
+        <v>18</v>
       </c>
       <c r="G47" s="8"/>
       <c r="H47" s="4"/>
@@ -5661,16 +5661,16 @@
         <v>0.65</v>
       </c>
       <c r="J47" s="4">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="K47" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L47" s="4">
         <v>0.71559633027522895</v>
       </c>
       <c r="M47" s="4">
-        <v>119.99353654242699</v>
+        <v>98.038134920634903</v>
       </c>
       <c r="N47" s="8"/>
       <c r="O47" s="4"/>
@@ -5678,16 +5678,16 @@
         <v>0.65</v>
       </c>
       <c r="Q47" s="4">
-        <v>195</v>
+        <v>0</v>
       </c>
       <c r="R47" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="S47" s="4">
         <v>0.73593073593073499</v>
       </c>
       <c r="T47" s="4">
-        <v>120.369285167334</v>
+        <v>108.406097337006</v>
       </c>
     </row>
     <row r="48" spans="1:20">
@@ -5696,16 +5696,16 @@
         <v>0.7</v>
       </c>
       <c r="C48" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D48" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E48" s="4">
         <v>0.94949494949494895</v>
       </c>
       <c r="F48" s="4">
-        <v>54.5485510380622</v>
+        <v>13</v>
       </c>
       <c r="G48" s="8"/>
       <c r="H48" s="4"/>
@@ -5713,7 +5713,7 @@
         <v>0.7</v>
       </c>
       <c r="J48" s="4">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="K48" s="4">
         <v>0</v>
@@ -5722,7 +5722,7 @@
         <v>0.72477064220183396</v>
       </c>
       <c r="M48" s="4">
-        <v>120.07921788434901</v>
+        <v>95.093134920634895</v>
       </c>
       <c r="N48" s="8"/>
       <c r="O48" s="4"/>
@@ -5730,7 +5730,7 @@
         <v>0.7</v>
       </c>
       <c r="Q48" s="4">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R48" s="4">
         <v>0</v>
@@ -5739,7 +5739,7 @@
         <v>0.73593073593073499</v>
       </c>
       <c r="T48" s="4">
-        <v>120.301142263759</v>
+        <v>106.301930670339</v>
       </c>
     </row>
     <row r="49" spans="1:20">
@@ -5748,7 +5748,7 @@
         <v>0.75</v>
       </c>
       <c r="C49" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D49" s="4">
         <v>0</v>
@@ -5757,7 +5757,7 @@
         <v>0.94949494949494895</v>
       </c>
       <c r="F49" s="4">
-        <v>54.532182398198501</v>
+        <v>9</v>
       </c>
       <c r="G49" s="8"/>
       <c r="H49" s="4"/>
@@ -5765,7 +5765,7 @@
         <v>0.75</v>
       </c>
       <c r="J49" s="4">
-        <v>31</v>
+        <v>0</v>
       </c>
       <c r="K49" s="4">
         <v>0</v>
@@ -5774,7 +5774,7 @@
         <v>0.72935779816513702</v>
       </c>
       <c r="M49" s="4">
-        <v>120.08893823629001</v>
+        <v>94.072569503146397</v>
       </c>
       <c r="N49" s="8"/>
       <c r="O49" s="4"/>
@@ -5782,7 +5782,7 @@
         <v>0.75</v>
       </c>
       <c r="Q49" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R49" s="4">
         <v>0</v>
@@ -5791,7 +5791,7 @@
         <v>0.73593073593073499</v>
       </c>
       <c r="T49" s="4">
-        <v>120.322522309356</v>
+        <v>106.246876417233</v>
       </c>
     </row>
     <row r="50" spans="1:20">
@@ -5800,7 +5800,7 @@
         <v>0.8</v>
       </c>
       <c r="C50" s="4">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="D50" s="4">
         <v>0</v>
@@ -5809,7 +5809,7 @@
         <v>0.959595959595959</v>
       </c>
       <c r="F50" s="4">
-        <v>54.768326758711297</v>
+        <v>7</v>
       </c>
       <c r="G50" s="8"/>
       <c r="H50" s="4"/>
@@ -5817,16 +5817,16 @@
         <v>0.8</v>
       </c>
       <c r="J50" s="4">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="K50" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="L50" s="4">
         <v>0.72935779816513702</v>
       </c>
       <c r="M50" s="4">
-        <v>120.05769421323799</v>
+        <v>93.844392006802707</v>
       </c>
       <c r="N50" s="8"/>
       <c r="O50" s="4"/>
@@ -5834,7 +5834,7 @@
         <v>0.8</v>
       </c>
       <c r="Q50" s="4">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="R50" s="4">
         <v>0</v>
@@ -5843,7 +5843,7 @@
         <v>0.74025974025973995</v>
       </c>
       <c r="T50" s="4">
-        <v>120.331348513984</v>
+        <v>103.251971749251</v>
       </c>
     </row>
     <row r="51" spans="1:20">
@@ -5852,7 +5852,7 @@
         <v>0.85</v>
       </c>
       <c r="C51" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D51" s="4">
         <v>0</v>
@@ -5861,7 +5861,7 @@
         <v>0.959595959595959</v>
       </c>
       <c r="F51" s="4">
-        <v>55.209035812672099</v>
+        <v>7</v>
       </c>
       <c r="G51" s="8"/>
       <c r="H51" s="4"/>
@@ -5869,7 +5869,7 @@
         <v>0.85</v>
       </c>
       <c r="J51" s="4">
-        <v>29</v>
+        <v>125</v>
       </c>
       <c r="K51" s="4">
         <v>0</v>
@@ -5878,7 +5878,7 @@
         <v>0.72935779816513702</v>
       </c>
       <c r="M51" s="4">
-        <v>120.14147222773001</v>
+        <v>90.910222505668898</v>
       </c>
       <c r="N51" s="8"/>
       <c r="O51" s="4"/>
@@ -5886,16 +5886,16 @@
         <v>0.85</v>
       </c>
       <c r="Q51" s="4">
-        <v>179</v>
+        <v>15</v>
       </c>
       <c r="R51" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="S51" s="4">
         <v>0.74458874458874402</v>
       </c>
       <c r="T51" s="4">
-        <v>120.354273504273</v>
+        <v>101.2635430839</v>
       </c>
     </row>
     <row r="52" spans="1:20">
@@ -5904,7 +5904,7 @@
         <v>0.9</v>
       </c>
       <c r="C52" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D52" s="4">
         <v>0</v>
@@ -5913,7 +5913,7 @@
         <v>0.959595959595959</v>
       </c>
       <c r="F52" s="4">
-        <v>55.7663673469388</v>
+        <v>7</v>
       </c>
       <c r="G52" s="8"/>
       <c r="H52" s="4"/>
@@ -5921,16 +5921,16 @@
         <v>0.9</v>
       </c>
       <c r="J52" s="4">
-        <v>285</v>
+        <v>0</v>
       </c>
       <c r="K52" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="L52" s="4">
         <v>0.73394495412843996</v>
       </c>
       <c r="M52" s="4">
-        <v>120.13918014665001</v>
+        <v>86.903347505668904</v>
       </c>
       <c r="N52" s="8"/>
       <c r="O52" s="4"/>
@@ -5938,7 +5938,7 @@
         <v>0.9</v>
       </c>
       <c r="Q52" s="4">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="R52" s="4">
         <v>0</v>
@@ -5947,7 +5947,7 @@
         <v>0.74891774891774798</v>
       </c>
       <c r="T52" s="4">
-        <v>120.411634001488</v>
+        <v>100.2635430839</v>
       </c>
     </row>
     <row r="53" spans="1:20">
@@ -5956,16 +5956,16 @@
         <v>0.95</v>
       </c>
       <c r="C53" s="4">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D53" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E53" s="4">
         <v>0.959595959595959</v>
       </c>
       <c r="F53" s="4">
-        <v>55.649291453615803</v>
+        <v>7</v>
       </c>
       <c r="G53" s="8"/>
       <c r="H53" s="4"/>
@@ -5973,7 +5973,7 @@
         <v>0.95</v>
       </c>
       <c r="J53" s="4">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="K53" s="4">
         <v>0</v>
@@ -5982,7 +5982,7 @@
         <v>0.73853211009174302</v>
       </c>
       <c r="M53" s="4">
-        <v>120.22369246463199</v>
+        <v>85.903347505668904</v>
       </c>
       <c r="N53" s="8"/>
       <c r="O53" s="4"/>
@@ -5990,7 +5990,7 @@
         <v>0.95</v>
       </c>
       <c r="Q53" s="4">
-        <v>16</v>
+        <v>126</v>
       </c>
       <c r="R53" s="4">
         <v>0</v>
@@ -5999,7 +5999,7 @@
         <v>0.74891774891774798</v>
       </c>
       <c r="T53" s="4">
-        <v>120.44584315293299</v>
+        <v>98.766944444444405</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Kolejne zadanie z weki, init
</commit_message>
<xml_diff>
--- a/weka-api-intro/excel z porownaniem.xlsx
+++ b/weka-api-intro/excel z porownaniem.xlsx
@@ -147,8 +147,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.8859857583527811E-2"/>
-          <c:y val="0.20861869743759509"/>
+          <c:x val="5.8859857583527804E-2"/>
+          <c:y val="0.20861869743759512"/>
           <c:w val="0.69853722326277934"/>
           <c:h val="0.66132778447739082"/>
         </c:manualLayout>
@@ -414,25 +414,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="81178624"/>
-        <c:axId val="81180160"/>
+        <c:axId val="91271168"/>
+        <c:axId val="91272704"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81178624"/>
+        <c:axId val="91271168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81180160"/>
+        <c:crossAx val="91272704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="81180160"/>
+        <c:axId val="91272704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -440,7 +440,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81178624"/>
+        <c:crossAx val="91271168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -453,7 +453,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -470,9 +470,9 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.8564304461942269E-2"/>
-          <c:y val="0.21002353579042063"/>
-          <c:w val="0.67025853018372716"/>
+          <c:x val="6.8564304461942283E-2"/>
+          <c:y val="0.21002353579042068"/>
+          <c:w val="0.67025853018372739"/>
           <c:h val="0.68831491134030798"/>
         </c:manualLayout>
       </c:layout>
@@ -794,25 +794,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="81186176"/>
-        <c:axId val="84878080"/>
+        <c:axId val="91278720"/>
+        <c:axId val="101393152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="81186176"/>
+        <c:axId val="91278720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84878080"/>
+        <c:crossAx val="101393152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84878080"/>
+        <c:axId val="101393152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -820,7 +820,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="81186176"/>
+        <c:crossAx val="91278720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -834,7 +834,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -851,10 +851,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="6.8564304461942269E-2"/>
+          <c:x val="6.8564304461942283E-2"/>
           <c:y val="0.16620506943674293"/>
-          <c:w val="0.67025853018372716"/>
-          <c:h val="0.73213337769398579"/>
+          <c:w val="0.67025853018372739"/>
+          <c:h val="0.7321333776939859"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1232,25 +1232,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="84908288"/>
-        <c:axId val="83107840"/>
+        <c:axId val="101423360"/>
+        <c:axId val="100806656"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="84908288"/>
+        <c:axId val="101423360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83107840"/>
+        <c:crossAx val="100806656"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83107840"/>
+        <c:axId val="100806656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1258,7 +1258,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="84908288"/>
+        <c:crossAx val="101423360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1272,7 +1272,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1291,8 +1291,8 @@
           <c:yMode val="edge"/>
           <c:x val="6.8564304461942283E-2"/>
           <c:y val="0.16620506943674293"/>
-          <c:w val="0.67025853018372761"/>
-          <c:h val="0.73213337769398601"/>
+          <c:w val="0.67025853018372772"/>
+          <c:h val="0.73213337769398612"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
@@ -1670,25 +1670,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83133184"/>
-        <c:axId val="83134720"/>
+        <c:axId val="100827904"/>
+        <c:axId val="100829440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83133184"/>
+        <c:axId val="100827904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83134720"/>
+        <c:crossAx val="100829440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83134720"/>
+        <c:axId val="100829440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1696,7 +1696,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83133184"/>
+        <c:crossAx val="100827904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1710,7 +1710,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000089" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000089" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1727,8 +1727,8 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.885985758352779E-2"/>
-          <c:y val="0.20861869743759517"/>
+          <c:x val="5.8859857583527783E-2"/>
+          <c:y val="0.20861869743759523"/>
           <c:w val="0.69853722326277934"/>
           <c:h val="0.66132778447739082"/>
         </c:manualLayout>
@@ -1994,25 +1994,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="83151872"/>
-        <c:axId val="85205760"/>
+        <c:axId val="100850688"/>
+        <c:axId val="101720832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="83151872"/>
+        <c:axId val="100850688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85205760"/>
+        <c:crossAx val="101720832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85205760"/>
+        <c:axId val="101720832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2020,7 +2020,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83151872"/>
+        <c:crossAx val="100850688"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2033,7 +2033,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -2051,7 +2051,7 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="5.8859857583527776E-2"/>
-          <c:y val="0.20861869743759526"/>
+          <c:y val="0.20861869743759529"/>
           <c:w val="0.69853722326277934"/>
           <c:h val="0.66132778447739082"/>
         </c:manualLayout>
@@ -2317,25 +2317,25 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="85218816"/>
-        <c:axId val="85220352"/>
+        <c:axId val="101733888"/>
+        <c:axId val="101735424"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="85218816"/>
+        <c:axId val="101733888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85220352"/>
+        <c:crossAx val="101735424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="85220352"/>
+        <c:axId val="101735424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2343,7 +2343,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="85218816"/>
+        <c:crossAx val="101733888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2356,7 +2356,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000056" l="0.70000000000000051" r="0.70000000000000051" t="0.75000000000000056" header="0.30000000000000027" footer="0.30000000000000027"/>
+    <c:pageMargins b="0.75000000000000078" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000078" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -2427,16 +2427,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>1057275</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2458,13 +2458,13 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>876300</xdr:colOff>
+      <xdr:colOff>857250</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>171450</xdr:colOff>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
@@ -2679,12 +2679,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.33281</cdr:x>
-      <cdr:y>0.09155</cdr:y>
+      <cdr:x>0.33437</cdr:x>
+      <cdr:y>0.09761</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.59844</cdr:x>
-      <cdr:y>0.14319</cdr:y>
+      <cdr:x>0.85938</cdr:x>
+      <cdr:y>0.16364</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2693,8 +2693,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2028825" y="371475"/>
-          <a:ext cx="1619250" cy="209550"/>
+          <a:off x="2038334" y="306815"/>
+          <a:ext cx="3200416" cy="207535"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2752,7 +2752,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="pl-PL" sz="1100"/>
-            <a:t>badges2 - błąd 0/1</a:t>
+            <a:t>badges2 - błąd 0/1 - liczba poprawnych</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -2768,12 +2768,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.38438</cdr:x>
-      <cdr:y>0.07042</cdr:y>
+      <cdr:x>0.14844</cdr:x>
+      <cdr:y>0.08685</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.67344</cdr:x>
-      <cdr:y>0.11737</cdr:y>
+      <cdr:x>0.65781</cdr:x>
+      <cdr:y>0.14319</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2782,8 +2782,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2343150" y="285750"/>
-          <a:ext cx="1762125" cy="190500"/>
+          <a:off x="904905" y="352415"/>
+          <a:ext cx="3105120" cy="228610"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2795,7 +2795,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="pl-PL" sz="1100"/>
-            <a:t>credit-a-mod - błąd 0/1</a:t>
+            <a:t>credit-a-mod - błąd 0/1 - liczba poprawnych</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -2811,12 +2811,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.38438</cdr:x>
-      <cdr:y>0.07042</cdr:y>
+      <cdr:x>0.18594</cdr:x>
+      <cdr:y>0.06103</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.67344</cdr:x>
-      <cdr:y>0.11737</cdr:y>
+      <cdr:x>0.74219</cdr:x>
+      <cdr:y>0.12911</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -2825,8 +2825,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="2343150" y="285750"/>
-          <a:ext cx="1762125" cy="190500"/>
+          <a:off x="1133505" y="247639"/>
+          <a:ext cx="3390870" cy="276235"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -2838,7 +2838,7 @@
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:r>
             <a:rPr lang="pl-PL" sz="1100"/>
-            <a:t>credit-a - błąd 0/1</a:t>
+            <a:t>credit-a - błąd 0/1 - liczba poprawnych</a:t>
           </a:r>
         </a:p>
         <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
@@ -3325,7 +3325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="F13" workbookViewId="0">
       <selection activeCell="Q55" sqref="Q55"/>
     </sheetView>
   </sheetViews>

</xml_diff>